<commit_message>
Lab03 - Added method searchForEmployee and added tests
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab01/Lab02_BBT_TCs_Form.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Utils\VSS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Faculta_Mark\Anul_3\Semestrul_2\VSS\Docs\cmir2085\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B2BB5F-BED9-4A09-B629-03094C25D233}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -17,17 +18,17 @@
     <sheet name="F01.BVA" sheetId="3" r:id="rId3"/>
     <sheet name="BBT-TCs" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="D22" authorId="0" shapeId="0">
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -46,12 +47,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="H36" authorId="0" shapeId="0">
+    <comment ref="H36" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -64,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K36" authorId="0" shapeId="0">
+    <comment ref="K36" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="115">
   <si>
     <t>do not print this form</t>
   </si>
@@ -282,9 +283,6 @@
   </si>
   <si>
     <t>Re-tested</t>
-  </si>
-  <si>
-    <t>not yet</t>
   </si>
   <si>
     <t>null</t>
@@ -546,17 +544,14 @@
     <t>"3300"</t>
   </si>
   <si>
-    <t>NullPointerException</t>
-  </si>
-  <si>
     <t>actual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1307,6 +1302,30 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1326,214 +1345,190 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1872,7 +1867,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF0066CC"/>
   </sheetPr>
@@ -1882,124 +1877,124 @@
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="17" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="14.25" customHeight="1">
+    <row r="1" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="2" spans="2:17" ht="14.25" customHeight="1">
-      <c r="L2" s="45" t="s">
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="54"/>
+    </row>
+    <row r="2" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L2" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-    </row>
-    <row r="3" spans="2:17" ht="14.25" customHeight="1">
-      <c r="L3" s="47" t="s">
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+    </row>
+    <row r="3" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L3" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="44"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="44"/>
-    </row>
-    <row r="4" spans="2:17" ht="14.25" customHeight="1">
+      <c r="M3" s="54"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="54"/>
+    </row>
+    <row r="4" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="47" t="s">
+      <c r="L4" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="44"/>
+      <c r="M4" s="54"/>
       <c r="N4" s="3"/>
       <c r="O4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="44"/>
-    </row>
-    <row r="5" spans="2:17" ht="14.25" customHeight="1">
+      <c r="P4" s="58"/>
+      <c r="Q4" s="54"/>
+    </row>
+    <row r="5" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:17" ht="14.25" customHeight="1">
+    <row r="6" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:17" ht="14.25" customHeight="1">
+    <row r="7" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="2:17" ht="14.25" customHeight="1">
+    <row r="8" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="2:17" ht="14.25" customHeight="1">
+    <row r="9" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="2:17" ht="14.25" customHeight="1">
+    <row r="10" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="2:17" ht="14.25" customHeight="1">
+    <row r="11" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="2:17" ht="14.25" customHeight="1">
+    <row r="12" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="2:17" ht="14.25" customHeight="1">
+    <row r="13" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:17" ht="14.25" customHeight="1">
+    <row r="14" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:17" ht="14.25" customHeight="1">
+    <row r="15" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" ht="14.25" customHeight="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="14.25" customHeight="1">
+    <row r="17" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
         <v>12</v>
       </c>
@@ -2016,7 +2011,7 @@
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="1:15" ht="14.25" customHeight="1">
+    <row r="18" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
         <v>13</v>
       </c>
@@ -2033,107 +2028,107 @@
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="1:15" ht="28.5" customHeight="1">
+    <row r="19" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
-      <c r="C19" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="41"/>
-      <c r="O19" s="41"/>
-    </row>
-    <row r="20" spans="1:15" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:15" ht="14.25" customHeight="1">
+      <c r="C19" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="51"/>
+    </row>
+    <row r="20" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="1:15" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:15" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:15" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:15" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:15" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:15" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:15" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:15" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:15" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:15" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:15" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="C19:O19"/>
@@ -2150,17 +2145,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFCC99"/>
   </sheetPr>
   <dimension ref="B1:O100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="N10" sqref="N10:O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="10.140625" customWidth="1"/>
@@ -2178,54 +2173,54 @@
     <col min="15" max="15" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="14.25" customHeight="1">
+    <row r="1" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="9"/>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="2" spans="2:15" ht="14.25" customHeight="1">
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="54"/>
+    </row>
+    <row r="2" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="2:15" ht="14.25" customHeight="1">
-      <c r="B3" s="59" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="44"/>
-    </row>
-    <row r="4" spans="2:15" ht="14.25" customHeight="1">
+    <row r="3" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="69" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="54"/>
+    </row>
+    <row r="4" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="2:15" ht="14.25" customHeight="1">
-      <c r="B5" s="60" t="s">
+    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="44"/>
-      <c r="G5" s="53" t="s">
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="54"/>
+      <c r="G5" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="44"/>
-    </row>
-    <row r="6" spans="2:15" ht="14.25" customHeight="1">
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="54"/>
+    </row>
+    <row r="6" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>16</v>
       </c>
@@ -2238,324 +2233,324 @@
       <c r="E6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="57" t="s">
+      <c r="G6" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="56" t="s">
+      <c r="H6" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="49" t="s">
+      <c r="I6" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="95"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="95"/>
-      <c r="M6" s="95"/>
-      <c r="N6" s="49" t="s">
+      <c r="J6" s="81"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="81"/>
+      <c r="N6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="O6" s="96"/>
-    </row>
-    <row r="7" spans="2:15" ht="14.25" customHeight="1">
+      <c r="O6" s="66"/>
+    </row>
+    <row r="7" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="11">
         <v>1</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="G7" s="97"/>
-      <c r="H7" s="97"/>
-      <c r="I7" s="10" t="s">
-        <v>75</v>
-      </c>
       <c r="J7" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="K7" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="L7" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="M7" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="M7" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="N7" s="49" t="s">
+      <c r="N7" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="O7" s="96"/>
-    </row>
-    <row r="8" spans="2:15" ht="14.25" customHeight="1">
+      <c r="O7" s="66"/>
+    </row>
+    <row r="8" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="11">
         <v>2</v>
       </c>
-      <c r="C8" s="55"/>
+      <c r="C8" s="76"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G8" s="10">
         <v>1</v>
       </c>
-      <c r="H8" s="99" t="s">
-        <v>92</v>
-      </c>
-      <c r="I8" s="99" t="s">
+      <c r="H8" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="I8" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="98"/>
-      <c r="K8" s="98"/>
-      <c r="L8" s="98"/>
-      <c r="M8" s="98">
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42">
         <v>3301</v>
       </c>
-      <c r="N8" s="52" t="b">
+      <c r="N8" s="67" t="b">
         <v>1</v>
       </c>
-      <c r="O8" s="96"/>
-    </row>
-    <row r="9" spans="2:15" ht="14.25" customHeight="1">
+      <c r="O8" s="66"/>
+    </row>
+    <row r="9" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="11">
         <v>3</v>
       </c>
-      <c r="C9" s="54" t="s">
-        <v>77</v>
+      <c r="C9" s="75" t="s">
+        <v>76</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" s="11"/>
       <c r="G9" s="10">
         <v>2</v>
       </c>
-      <c r="H9" s="98" t="s">
-        <v>93</v>
-      </c>
-      <c r="I9" s="99" t="s">
-        <v>78</v>
-      </c>
-      <c r="J9" s="98"/>
-      <c r="K9" s="98"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="98">
+      <c r="H9" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42">
         <v>3301</v>
       </c>
-      <c r="N9" s="52" t="b">
+      <c r="N9" s="67" t="b">
         <v>1</v>
       </c>
-      <c r="O9" s="96"/>
-    </row>
-    <row r="10" spans="2:15" ht="14.25" customHeight="1">
+      <c r="O9" s="66"/>
+    </row>
+    <row r="10" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="11">
         <v>4</v>
       </c>
-      <c r="C10" s="55"/>
+      <c r="C10" s="76"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G10" s="13">
         <v>3</v>
       </c>
-      <c r="H10" s="98" t="s">
-        <v>94</v>
-      </c>
-      <c r="I10" s="98" t="s">
-        <v>60</v>
+      <c r="H10" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" s="42" t="s">
+        <v>59</v>
       </c>
       <c r="J10" s="17"/>
-      <c r="K10" s="98"/>
-      <c r="L10" s="98"/>
-      <c r="M10" s="98">
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42">
         <v>3301</v>
       </c>
-      <c r="N10" s="118" t="s">
-        <v>115</v>
-      </c>
-      <c r="O10" s="101"/>
-    </row>
-    <row r="11" spans="2:15">
+      <c r="N10" s="63" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" s="64"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="11">
         <v>5</v>
       </c>
-      <c r="C11" s="54" t="s">
-        <v>82</v>
+      <c r="C11" s="75" t="s">
+        <v>81</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E11" s="11"/>
       <c r="G11" s="13">
         <v>4</v>
       </c>
-      <c r="H11" s="98" t="s">
-        <v>95</v>
-      </c>
-      <c r="I11" s="98" t="s">
-        <v>80</v>
-      </c>
-      <c r="J11" s="98"/>
-      <c r="K11" s="98"/>
-      <c r="L11" s="98"/>
-      <c r="M11" s="98">
+      <c r="H11" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42">
         <v>3300</v>
       </c>
-      <c r="N11" s="118" t="b">
+      <c r="N11" s="63" t="b">
         <v>0</v>
       </c>
-      <c r="O11" s="101"/>
-    </row>
-    <row r="12" spans="2:15" ht="14.25" customHeight="1">
+      <c r="O11" s="64"/>
+    </row>
+    <row r="12" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="11">
         <v>6</v>
       </c>
-      <c r="C12" s="55"/>
+      <c r="C12" s="76"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G12" s="14">
         <v>5</v>
       </c>
-      <c r="H12" s="98" t="s">
-        <v>96</v>
-      </c>
-      <c r="I12" s="98" t="s">
+      <c r="H12" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="I12" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="98"/>
-      <c r="K12" s="98"/>
-      <c r="L12" s="98"/>
-      <c r="M12" s="98">
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42">
         <v>3300</v>
       </c>
-      <c r="N12" s="118" t="b">
+      <c r="N12" s="63" t="b">
         <v>0</v>
       </c>
-      <c r="O12" s="101"/>
-    </row>
-    <row r="13" spans="2:15" ht="14.25" customHeight="1">
+      <c r="O12" s="64"/>
+    </row>
+    <row r="13" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
         <v>7</v>
       </c>
-      <c r="C13" s="54" t="s">
-        <v>106</v>
+      <c r="C13" s="75" t="s">
+        <v>105</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E13" s="11"/>
       <c r="G13" s="14">
         <v>6</v>
       </c>
-      <c r="H13" s="98" t="s">
-        <v>97</v>
-      </c>
-      <c r="I13" s="99" t="s">
-        <v>63</v>
-      </c>
-      <c r="J13" s="98"/>
-      <c r="K13" s="99"/>
-      <c r="L13" s="98"/>
-      <c r="M13" s="98" t="s">
-        <v>114</v>
-      </c>
-      <c r="N13" s="118" t="b">
+      <c r="H13" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="I13" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="42"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="N13" s="63" t="b">
         <v>0</v>
       </c>
-      <c r="O13" s="101"/>
-    </row>
-    <row r="14" spans="2:15" ht="14.25" customHeight="1">
+      <c r="O13" s="64"/>
+    </row>
+    <row r="14" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
         <v>8</v>
       </c>
-      <c r="C14" s="55"/>
+      <c r="C14" s="76"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G14" s="15">
         <v>7</v>
       </c>
-      <c r="H14" s="99" t="s">
-        <v>95</v>
-      </c>
-      <c r="I14" s="99" t="s">
-        <v>80</v>
-      </c>
-      <c r="J14" s="98"/>
-      <c r="K14" s="98"/>
-      <c r="L14" s="98"/>
-      <c r="M14" s="98">
+      <c r="H14" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42">
         <v>12000</v>
       </c>
-      <c r="N14" s="118" t="b">
+      <c r="N14" s="63" t="b">
         <v>0</v>
       </c>
-      <c r="O14" s="101"/>
-    </row>
-    <row r="15" spans="2:15" ht="14.25" customHeight="1">
+      <c r="O14" s="64"/>
+    </row>
+    <row r="15" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="11">
         <v>9</v>
       </c>
-      <c r="C15" s="109" t="s">
+      <c r="C15" s="71" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>84</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>85</v>
       </c>
       <c r="E15" s="11"/>
       <c r="G15" s="15">
         <v>8</v>
       </c>
-      <c r="H15" s="99" t="s">
-        <v>98</v>
-      </c>
-      <c r="I15" s="99" t="s">
-        <v>81</v>
+      <c r="H15" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="43" t="s">
+        <v>80</v>
       </c>
       <c r="J15" s="24"/>
-      <c r="K15" s="100"/>
+      <c r="K15" s="44"/>
       <c r="L15" s="24"/>
-      <c r="M15" s="100">
+      <c r="M15" s="44">
         <v>8000</v>
       </c>
-      <c r="N15" s="118" t="b">
+      <c r="N15" s="63" t="b">
         <v>0</v>
       </c>
-      <c r="O15" s="101"/>
-    </row>
-    <row r="16" spans="2:15" ht="14.25" customHeight="1">
+      <c r="O15" s="64"/>
+    </row>
+    <row r="16" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
         <v>10</v>
       </c>
-      <c r="C16" s="110"/>
+      <c r="C16" s="72"/>
       <c r="D16" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" s="102"/>
+        <v>85</v>
+      </c>
+      <c r="E16" s="45"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="99"/>
-      <c r="I16" s="99"/>
-      <c r="J16" s="98"/>
-      <c r="K16" s="98"/>
-      <c r="L16" s="98"/>
-      <c r="M16" s="98"/>
-      <c r="N16" s="112"/>
-      <c r="O16" s="113"/>
-    </row>
-    <row r="17" spans="2:15" ht="14.25" customHeight="1">
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="62"/>
+    </row>
+    <row r="17" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
         <v>11</v>
       </c>
-      <c r="C17" s="110"/>
+      <c r="C17" s="72"/>
       <c r="D17" s="11"/>
-      <c r="E17" s="102" t="s">
-        <v>87</v>
+      <c r="E17" s="45" t="s">
+        <v>86</v>
       </c>
       <c r="G17" s="15"/>
       <c r="H17" s="16"/>
@@ -2564,11 +2559,11 @@
       <c r="K17" s="16"/>
       <c r="L17" s="16"/>
       <c r="M17" s="16"/>
-      <c r="N17" s="116"/>
-      <c r="O17" s="117"/>
-    </row>
-    <row r="18" spans="2:15" ht="14.25" customHeight="1">
-      <c r="C18" s="111"/>
+      <c r="N17" s="59"/>
+      <c r="O17" s="60"/>
+    </row>
+    <row r="18" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="73"/>
       <c r="D18" t="s">
         <v>27</v>
       </c>
@@ -2579,10 +2574,10 @@
       <c r="K18" s="16"/>
       <c r="L18" s="16"/>
       <c r="M18" s="16"/>
-      <c r="N18" s="116"/>
-      <c r="O18" s="117"/>
-    </row>
-    <row r="19" spans="2:15" ht="14.25" customHeight="1">
+      <c r="N18" s="59"/>
+      <c r="O18" s="60"/>
+    </row>
+    <row r="19" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="9"/>
       <c r="G19" s="10"/>
       <c r="H19" s="12"/>
@@ -2591,270 +2586,252 @@
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="44"/>
-    </row>
-    <row r="20" spans="2:15" ht="14.25" customHeight="1">
+      <c r="N19" s="77"/>
+      <c r="O19" s="54"/>
+    </row>
+    <row r="20" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="9"/>
     </row>
-    <row r="21" spans="2:15" ht="14.25" customHeight="1">
+    <row r="21" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="9"/>
     </row>
-    <row r="22" spans="2:15" ht="14.25" customHeight="1">
+    <row r="22" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="9"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="41"/>
-    </row>
-    <row r="23" spans="2:15" ht="14.25" customHeight="1">
+      <c r="F22" s="68"/>
+      <c r="G22" s="51"/>
+    </row>
+    <row r="23" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="2:15" ht="14.25" customHeight="1">
+    <row r="24" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="2:15" ht="14.25" customHeight="1">
+    <row r="25" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="9"/>
     </row>
-    <row r="26" spans="2:15" ht="14.25" customHeight="1">
+    <row r="26" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="9"/>
     </row>
-    <row r="27" spans="2:15" ht="14.25" customHeight="1">
+    <row r="27" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="9"/>
     </row>
-    <row r="28" spans="2:15" ht="14.25" customHeight="1">
+    <row r="28" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="9"/>
     </row>
-    <row r="29" spans="2:15" ht="14.25" customHeight="1">
+    <row r="29" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="9"/>
     </row>
-    <row r="30" spans="2:15" ht="14.25" customHeight="1">
+    <row r="30" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="9"/>
     </row>
-    <row r="31" spans="2:15" ht="14.25" customHeight="1">
+    <row r="31" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="9"/>
     </row>
-    <row r="32" spans="2:15" ht="14.25" customHeight="1">
+    <row r="32" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C32" s="9"/>
     </row>
-    <row r="33" spans="3:3" ht="14.25" customHeight="1">
+    <row r="33" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C33" s="9"/>
     </row>
-    <row r="34" spans="3:3" ht="14.25" customHeight="1">
+    <row r="34" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="9"/>
     </row>
-    <row r="35" spans="3:3" ht="14.25" customHeight="1">
+    <row r="35" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="9"/>
     </row>
-    <row r="36" spans="3:3" ht="14.25" customHeight="1">
+    <row r="36" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="9"/>
     </row>
-    <row r="37" spans="3:3" ht="14.25" customHeight="1">
+    <row r="37" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="9"/>
     </row>
-    <row r="38" spans="3:3" ht="14.25" customHeight="1">
+    <row r="38" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="9"/>
     </row>
-    <row r="39" spans="3:3" ht="14.25" customHeight="1">
+    <row r="39" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="9"/>
     </row>
-    <row r="40" spans="3:3" ht="14.25" customHeight="1">
+    <row r="40" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="9"/>
     </row>
-    <row r="41" spans="3:3" ht="14.25" customHeight="1">
+    <row r="41" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="9"/>
     </row>
-    <row r="42" spans="3:3" ht="14.25" customHeight="1">
+    <row r="42" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C42" s="9"/>
     </row>
-    <row r="43" spans="3:3" ht="14.25" customHeight="1">
+    <row r="43" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C43" s="9"/>
     </row>
-    <row r="44" spans="3:3" ht="14.25" customHeight="1">
+    <row r="44" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C44" s="9"/>
     </row>
-    <row r="45" spans="3:3" ht="14.25" customHeight="1">
+    <row r="45" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C45" s="9"/>
     </row>
-    <row r="46" spans="3:3" ht="14.25" customHeight="1">
+    <row r="46" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C46" s="9"/>
     </row>
-    <row r="47" spans="3:3" ht="14.25" customHeight="1">
+    <row r="47" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C47" s="9"/>
     </row>
-    <row r="48" spans="3:3" ht="14.25" customHeight="1">
+    <row r="48" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C48" s="9"/>
     </row>
-    <row r="49" spans="3:3" ht="14.25" customHeight="1">
+    <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C49" s="9"/>
     </row>
-    <row r="50" spans="3:3" ht="14.25" customHeight="1">
+    <row r="50" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C50" s="9"/>
     </row>
-    <row r="51" spans="3:3" ht="14.25" customHeight="1">
+    <row r="51" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C51" s="9"/>
     </row>
-    <row r="52" spans="3:3" ht="14.25" customHeight="1">
+    <row r="52" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C52" s="9"/>
     </row>
-    <row r="53" spans="3:3" ht="14.25" customHeight="1">
+    <row r="53" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C53" s="9"/>
     </row>
-    <row r="54" spans="3:3" ht="14.25" customHeight="1">
+    <row r="54" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C54" s="9"/>
     </row>
-    <row r="55" spans="3:3" ht="14.25" customHeight="1">
+    <row r="55" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C55" s="9"/>
     </row>
-    <row r="56" spans="3:3" ht="14.25" customHeight="1">
+    <row r="56" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C56" s="9"/>
     </row>
-    <row r="57" spans="3:3" ht="14.25" customHeight="1">
+    <row r="57" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C57" s="9"/>
     </row>
-    <row r="58" spans="3:3" ht="14.25" customHeight="1">
+    <row r="58" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C58" s="9"/>
     </row>
-    <row r="59" spans="3:3" ht="14.25" customHeight="1">
+    <row r="59" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C59" s="9"/>
     </row>
-    <row r="60" spans="3:3" ht="14.25" customHeight="1">
+    <row r="60" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C60" s="9"/>
     </row>
-    <row r="61" spans="3:3" ht="14.25" customHeight="1">
+    <row r="61" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C61" s="9"/>
     </row>
-    <row r="62" spans="3:3" ht="14.25" customHeight="1">
+    <row r="62" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C62" s="9"/>
     </row>
-    <row r="63" spans="3:3" ht="14.25" customHeight="1">
+    <row r="63" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C63" s="9"/>
     </row>
-    <row r="64" spans="3:3" ht="14.25" customHeight="1">
+    <row r="64" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C64" s="9"/>
     </row>
-    <row r="65" spans="3:3" ht="14.25" customHeight="1">
+    <row r="65" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C65" s="9"/>
     </row>
-    <row r="66" spans="3:3" ht="14.25" customHeight="1">
+    <row r="66" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C66" s="9"/>
     </row>
-    <row r="67" spans="3:3" ht="14.25" customHeight="1">
+    <row r="67" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="9"/>
     </row>
-    <row r="68" spans="3:3" ht="14.25" customHeight="1">
+    <row r="68" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C68" s="9"/>
     </row>
-    <row r="69" spans="3:3" ht="14.25" customHeight="1">
+    <row r="69" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C69" s="9"/>
     </row>
-    <row r="70" spans="3:3" ht="14.25" customHeight="1">
+    <row r="70" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C70" s="9"/>
     </row>
-    <row r="71" spans="3:3" ht="14.25" customHeight="1">
+    <row r="71" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C71" s="9"/>
     </row>
-    <row r="72" spans="3:3" ht="14.25" customHeight="1">
+    <row r="72" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C72" s="9"/>
     </row>
-    <row r="73" spans="3:3" ht="14.25" customHeight="1">
+    <row r="73" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C73" s="9"/>
     </row>
-    <row r="74" spans="3:3" ht="14.25" customHeight="1">
+    <row r="74" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C74" s="9"/>
     </row>
-    <row r="75" spans="3:3" ht="14.25" customHeight="1">
+    <row r="75" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C75" s="9"/>
     </row>
-    <row r="76" spans="3:3" ht="14.25" customHeight="1">
+    <row r="76" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C76" s="9"/>
     </row>
-    <row r="77" spans="3:3" ht="14.25" customHeight="1">
+    <row r="77" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C77" s="9"/>
     </row>
-    <row r="78" spans="3:3" ht="14.25" customHeight="1">
+    <row r="78" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C78" s="9"/>
     </row>
-    <row r="79" spans="3:3" ht="14.25" customHeight="1">
+    <row r="79" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C79" s="9"/>
     </row>
-    <row r="80" spans="3:3" ht="14.25" customHeight="1">
+    <row r="80" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C80" s="9"/>
     </row>
-    <row r="81" spans="3:3" ht="14.25" customHeight="1">
+    <row r="81" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C81" s="9"/>
     </row>
-    <row r="82" spans="3:3" ht="14.25" customHeight="1">
+    <row r="82" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C82" s="9"/>
     </row>
-    <row r="83" spans="3:3" ht="14.25" customHeight="1">
+    <row r="83" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C83" s="9"/>
     </row>
-    <row r="84" spans="3:3" ht="14.25" customHeight="1">
+    <row r="84" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C84" s="9"/>
     </row>
-    <row r="85" spans="3:3" ht="14.25" customHeight="1">
+    <row r="85" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C85" s="9"/>
     </row>
-    <row r="86" spans="3:3" ht="14.25" customHeight="1">
+    <row r="86" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C86" s="9"/>
     </row>
-    <row r="87" spans="3:3" ht="14.25" customHeight="1">
+    <row r="87" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C87" s="9"/>
     </row>
-    <row r="88" spans="3:3" ht="14.25" customHeight="1">
+    <row r="88" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C88" s="9"/>
     </row>
-    <row r="89" spans="3:3" ht="14.25" customHeight="1">
+    <row r="89" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C89" s="9"/>
     </row>
-    <row r="90" spans="3:3" ht="14.25" customHeight="1">
+    <row r="90" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C90" s="9"/>
     </row>
-    <row r="91" spans="3:3" ht="14.25" customHeight="1">
+    <row r="91" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C91" s="9"/>
     </row>
-    <row r="92" spans="3:3" ht="14.25" customHeight="1">
+    <row r="92" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C92" s="9"/>
     </row>
-    <row r="93" spans="3:3" ht="14.25" customHeight="1">
+    <row r="93" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C93" s="9"/>
     </row>
-    <row r="94" spans="3:3" ht="14.25" customHeight="1">
+    <row r="94" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C94" s="9"/>
     </row>
-    <row r="95" spans="3:3" ht="14.25" customHeight="1">
+    <row r="95" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C95" s="9"/>
     </row>
-    <row r="96" spans="3:3" ht="14.25" customHeight="1">
+    <row r="96" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C96" s="9"/>
     </row>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="G5:O5"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
     <mergeCell ref="N19:O19"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="G6:G7"/>
@@ -2864,6 +2841,24 @@
     <mergeCell ref="N11:O11"/>
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="G5:O5"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2871,17 +2866,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFCC99"/>
   </sheetPr>
   <dimension ref="B1:R100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="P9" sqref="P9:Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
@@ -2903,52 +2898,52 @@
     <col min="18" max="18" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="14.25" customHeight="1">
+    <row r="1" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="9"/>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="2" spans="2:17" ht="14.25" customHeight="1"/>
-    <row r="3" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B3" s="59" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="44"/>
-    </row>
-    <row r="4" spans="2:17" ht="14.25" customHeight="1"/>
-    <row r="5" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B5" s="67" t="s">
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="54"/>
+    </row>
+    <row r="2" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="69" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="54"/>
+    </row>
+    <row r="4" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="54"/>
       <c r="E5" s="17"/>
-      <c r="G5" s="53" t="s">
+      <c r="G5" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="44"/>
-    </row>
-    <row r="6" spans="2:17" ht="14.25" customHeight="1">
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="53"/>
+      <c r="Q5" s="54"/>
+    </row>
+    <row r="6" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>30</v>
       </c>
@@ -2959,70 +2954,70 @@
         <v>28</v>
       </c>
       <c r="E6" s="18"/>
-      <c r="G6" s="57" t="s">
+      <c r="G6" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="57" t="s">
+      <c r="H6" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="57" t="s">
+      <c r="I6" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="56" t="s">
+      <c r="J6" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="66" t="s">
+      <c r="K6" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="43"/>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="66" t="s">
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="53"/>
+      <c r="O6" s="53"/>
+      <c r="P6" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="Q6" s="44"/>
-    </row>
-    <row r="7" spans="2:17" ht="28.5" customHeight="1">
-      <c r="B7" s="54">
+      <c r="Q6" s="54"/>
+    </row>
+    <row r="7" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="75">
         <v>1</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="83" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="E7" s="9"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="P7" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="54"/>
+    </row>
+    <row r="8" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="40" t="s">
         <v>100</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="M7" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="N7" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="O7" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="P7" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q7" s="44"/>
-    </row>
-    <row r="8" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="93" t="s">
-        <v>101</v>
       </c>
       <c r="E8" s="9"/>
       <c r="G8" s="10">
@@ -3031,13 +3026,13 @@
       <c r="H8" s="20">
         <v>1</v>
       </c>
-      <c r="I8" s="100" t="s">
-        <v>61</v>
-      </c>
-      <c r="J8" s="100" t="s">
+      <c r="I8" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="K8" s="94" t="s">
+      <c r="K8" s="41" t="s">
         <v>26</v>
       </c>
       <c r="L8" s="22"/>
@@ -3046,16 +3041,16 @@
       <c r="O8" s="22">
         <v>3302</v>
       </c>
-      <c r="P8" s="108" t="b">
+      <c r="P8" s="85" t="b">
         <v>0</v>
       </c>
-      <c r="Q8" s="44"/>
-    </row>
-    <row r="9" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B9" s="62"/>
-      <c r="C9" s="62"/>
+      <c r="Q8" s="54"/>
+    </row>
+    <row r="9" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="82"/>
+      <c r="C9" s="82"/>
       <c r="D9" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E9" s="9"/>
       <c r="G9" s="15">
@@ -3064,14 +3059,14 @@
       <c r="H9" s="23">
         <v>2</v>
       </c>
-      <c r="I9" s="106" t="s">
+      <c r="I9" s="46" t="s">
         <v>36</v>
       </c>
       <c r="J9" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="107" t="s">
-        <v>60</v>
+      <c r="K9" s="47" t="s">
+        <v>59</v>
       </c>
       <c r="L9" s="22"/>
       <c r="M9" s="22"/>
@@ -3079,16 +3074,16 @@
       <c r="O9" s="22">
         <v>3302</v>
       </c>
-      <c r="P9" s="108" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q9" s="44"/>
-    </row>
-    <row r="10" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
+      <c r="P9" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="54"/>
+    </row>
+    <row r="10" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
       <c r="D10" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E10" s="9"/>
       <c r="G10" s="10">
@@ -3097,11 +3092,11 @@
       <c r="H10" s="20">
         <v>3</v>
       </c>
-      <c r="I10" s="123" t="s">
-        <v>62</v>
-      </c>
-      <c r="J10" s="100" t="s">
-        <v>66</v>
+      <c r="I10" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="44" t="s">
+        <v>65</v>
       </c>
       <c r="K10" s="26" t="s">
         <v>38</v>
@@ -3112,16 +3107,16 @@
       <c r="O10" s="22">
         <v>3302</v>
       </c>
-      <c r="P10" s="92" t="b">
+      <c r="P10" s="86" t="b">
         <v>1</v>
       </c>
-      <c r="Q10" s="44"/>
-    </row>
-    <row r="11" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B11" s="62"/>
-      <c r="C11" s="62"/>
+      <c r="Q10" s="54"/>
+    </row>
+    <row r="11" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="82"/>
+      <c r="C11" s="82"/>
       <c r="D11" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E11" s="9"/>
       <c r="G11" s="10">
@@ -3130,11 +3125,11 @@
       <c r="H11" s="20">
         <v>4</v>
       </c>
-      <c r="I11" s="123" t="s">
-        <v>62</v>
-      </c>
-      <c r="J11" s="100" t="s">
-        <v>66</v>
+      <c r="I11" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="44" t="s">
+        <v>65</v>
       </c>
       <c r="K11" s="26" t="s">
         <v>39</v>
@@ -3145,16 +3140,16 @@
       <c r="O11" s="22">
         <v>3302</v>
       </c>
-      <c r="P11" s="92" t="b">
+      <c r="P11" s="86" t="b">
         <v>1</v>
       </c>
-      <c r="Q11" s="44"/>
-    </row>
-    <row r="12" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B12" s="55"/>
-      <c r="C12" s="55"/>
+      <c r="Q11" s="54"/>
+    </row>
+    <row r="12" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
       <c r="D12" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E12" s="9"/>
       <c r="G12" s="10">
@@ -3163,11 +3158,11 @@
       <c r="H12" s="20">
         <v>5</v>
       </c>
-      <c r="I12" s="123" t="s">
-        <v>62</v>
-      </c>
-      <c r="J12" s="100" t="s">
-        <v>66</v>
+      <c r="I12" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" s="44" t="s">
+        <v>65</v>
       </c>
       <c r="K12" s="26" t="s">
         <v>40</v>
@@ -3178,20 +3173,20 @@
       <c r="O12" s="22">
         <v>3302</v>
       </c>
-      <c r="P12" s="92" t="b">
+      <c r="P12" s="86" t="b">
         <v>1</v>
       </c>
-      <c r="Q12" s="44"/>
-    </row>
-    <row r="13" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B13" s="54">
+      <c r="Q12" s="54"/>
+    </row>
+    <row r="13" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="75">
         <v>2</v>
       </c>
-      <c r="C13" s="105" t="s">
+      <c r="C13" s="90" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="40" t="s">
         <v>106</v>
-      </c>
-      <c r="D13" s="93" t="s">
-        <v>107</v>
       </c>
       <c r="E13" s="9"/>
       <c r="G13" s="15">
@@ -3200,8 +3195,8 @@
       <c r="H13" s="23">
         <v>6</v>
       </c>
-      <c r="I13" s="106" t="s">
-        <v>65</v>
+      <c r="I13" s="46" t="s">
+        <v>64</v>
       </c>
       <c r="J13" s="24" t="s">
         <v>37</v>
@@ -3215,16 +3210,16 @@
       <c r="O13" s="22">
         <v>3302</v>
       </c>
-      <c r="P13" s="50" t="b">
+      <c r="P13" s="94" t="b">
         <v>0</v>
       </c>
-      <c r="Q13" s="44"/>
-    </row>
-    <row r="14" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B14" s="103"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="93" t="s">
-        <v>108</v>
+      <c r="Q13" s="54"/>
+    </row>
+    <row r="14" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="88"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="40" t="s">
+        <v>107</v>
       </c>
       <c r="E14" s="9"/>
       <c r="G14" s="10">
@@ -3233,31 +3228,31 @@
       <c r="H14" s="20">
         <v>7</v>
       </c>
-      <c r="I14" s="106" t="s">
-        <v>67</v>
-      </c>
-      <c r="J14" s="100" t="s">
+      <c r="I14" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="K14" s="94" t="s">
-        <v>80</v>
+      <c r="K14" s="41" t="s">
+        <v>79</v>
       </c>
       <c r="L14" s="22"/>
       <c r="M14" s="22"/>
       <c r="N14" s="22"/>
-      <c r="O14" s="122">
+      <c r="O14" s="48">
         <v>3300</v>
       </c>
-      <c r="P14" s="50" t="b">
+      <c r="P14" s="94" t="b">
         <v>0</v>
       </c>
-      <c r="Q14" s="44"/>
-    </row>
-    <row r="15" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B15" s="103"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="93" t="s">
-        <v>109</v>
+      <c r="Q14" s="54"/>
+    </row>
+    <row r="15" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="88"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="40" t="s">
+        <v>108</v>
       </c>
       <c r="E15" s="9"/>
       <c r="G15" s="10">
@@ -3266,14 +3261,14 @@
       <c r="H15" s="20">
         <v>8</v>
       </c>
-      <c r="I15" s="123" t="s">
-        <v>64</v>
-      </c>
-      <c r="J15" s="100" t="s">
-        <v>66</v>
-      </c>
-      <c r="K15" s="94" t="s">
-        <v>80</v>
+      <c r="I15" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" s="41" t="s">
+        <v>79</v>
       </c>
       <c r="L15" s="22"/>
       <c r="M15" s="22"/>
@@ -3281,16 +3276,16 @@
       <c r="O15" s="22">
         <v>3301</v>
       </c>
-      <c r="P15" s="92" t="b">
+      <c r="P15" s="86" t="b">
         <v>1</v>
       </c>
-      <c r="Q15" s="44"/>
-    </row>
-    <row r="16" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B16" s="103"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="93" t="s">
-        <v>110</v>
+      <c r="Q15" s="54"/>
+    </row>
+    <row r="16" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="88"/>
+      <c r="C16" s="82"/>
+      <c r="D16" s="40" t="s">
+        <v>109</v>
       </c>
       <c r="E16" s="9"/>
       <c r="G16" s="10">
@@ -3299,14 +3294,14 @@
       <c r="H16" s="20">
         <v>9</v>
       </c>
-      <c r="I16" s="123" t="s">
-        <v>64</v>
-      </c>
-      <c r="J16" s="100" t="s">
-        <v>66</v>
-      </c>
-      <c r="K16" s="94" t="s">
-        <v>80</v>
+      <c r="I16" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="K16" s="41" t="s">
+        <v>79</v>
       </c>
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
@@ -3314,16 +3309,16 @@
       <c r="O16" s="22">
         <v>3302</v>
       </c>
-      <c r="P16" s="92" t="b">
+      <c r="P16" s="86" t="b">
         <v>1</v>
       </c>
-      <c r="Q16" s="44"/>
-    </row>
-    <row r="17" spans="2:18" ht="14.25" customHeight="1">
-      <c r="B17" s="103"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="93" t="s">
-        <v>111</v>
+      <c r="Q16" s="54"/>
+    </row>
+    <row r="17" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="88"/>
+      <c r="C17" s="82"/>
+      <c r="D17" s="40" t="s">
+        <v>110</v>
       </c>
       <c r="E17" s="9"/>
       <c r="G17" s="10">
@@ -3332,14 +3327,14 @@
       <c r="H17" s="20">
         <v>10</v>
       </c>
-      <c r="I17" s="123" t="s">
-        <v>64</v>
-      </c>
-      <c r="J17" s="100" t="s">
-        <v>66</v>
-      </c>
-      <c r="K17" s="94" t="s">
-        <v>80</v>
+      <c r="I17" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="K17" s="41" t="s">
+        <v>79</v>
       </c>
       <c r="L17" s="22"/>
       <c r="M17" s="22"/>
@@ -3347,16 +3342,16 @@
       <c r="O17" s="22">
         <v>11998</v>
       </c>
-      <c r="P17" s="92" t="b">
+      <c r="P17" s="86" t="b">
         <v>1</v>
       </c>
-      <c r="Q17" s="44"/>
-    </row>
-    <row r="18" spans="2:18" ht="14.25" customHeight="1">
-      <c r="B18" s="104"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="93" t="s">
-        <v>112</v>
+      <c r="Q17" s="54"/>
+    </row>
+    <row r="18" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="89"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="40" t="s">
+        <v>111</v>
       </c>
       <c r="E18" s="9"/>
       <c r="G18" s="10">
@@ -3365,14 +3360,14 @@
       <c r="H18" s="20">
         <v>11</v>
       </c>
-      <c r="I18" s="123" t="s">
-        <v>64</v>
-      </c>
-      <c r="J18" s="100" t="s">
-        <v>66</v>
-      </c>
-      <c r="K18" s="94" t="s">
-        <v>80</v>
+      <c r="I18" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="J18" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="K18" s="41" t="s">
+        <v>79</v>
       </c>
       <c r="L18" s="22"/>
       <c r="M18" s="22"/>
@@ -3380,19 +3375,19 @@
       <c r="O18" s="22">
         <v>11999</v>
       </c>
-      <c r="P18" s="92" t="b">
+      <c r="P18" s="86" t="b">
         <v>1</v>
       </c>
-      <c r="Q18" s="44"/>
-    </row>
-    <row r="19" spans="2:18" ht="14.25" customHeight="1">
-      <c r="B19" s="54">
+      <c r="Q18" s="54"/>
+    </row>
+    <row r="19" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="75">
         <v>3</v>
       </c>
-      <c r="C19" s="105" t="s">
+      <c r="C19" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="93" t="s">
+      <c r="D19" s="40" t="s">
         <v>25</v>
       </c>
       <c r="E19" s="9"/>
@@ -3402,30 +3397,30 @@
       <c r="H19" s="20">
         <v>12</v>
       </c>
-      <c r="I19" s="106" t="s">
-        <v>68</v>
-      </c>
-      <c r="J19" s="100" t="s">
+      <c r="I19" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="K19" s="94" t="s">
-        <v>80</v>
+      <c r="K19" s="41" t="s">
+        <v>79</v>
       </c>
       <c r="L19" s="22"/>
       <c r="M19" s="22"/>
       <c r="N19" s="22"/>
-      <c r="O19" s="122">
+      <c r="O19" s="48">
         <v>12000</v>
       </c>
-      <c r="P19" s="108" t="b">
+      <c r="P19" s="85" t="b">
         <v>0</v>
       </c>
-      <c r="Q19" s="44"/>
-    </row>
-    <row r="20" spans="2:18" ht="14.25" customHeight="1">
-      <c r="B20" s="62"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="93" t="s">
+      <c r="Q19" s="54"/>
+    </row>
+    <row r="20" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="82"/>
+      <c r="C20" s="82"/>
+      <c r="D20" s="40" t="s">
         <v>25</v>
       </c>
       <c r="E20" s="9"/>
@@ -3440,13 +3435,13 @@
       <c r="M20" s="22"/>
       <c r="N20" s="22"/>
       <c r="O20" s="22"/>
-      <c r="P20" s="61"/>
-      <c r="Q20" s="44"/>
-    </row>
-    <row r="21" spans="2:18" ht="14.25" customHeight="1">
-      <c r="B21" s="62"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="93" t="s">
+      <c r="P20" s="93"/>
+      <c r="Q20" s="54"/>
+    </row>
+    <row r="21" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="82"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="40" t="s">
         <v>25</v>
       </c>
       <c r="E21" s="9"/>
@@ -3461,13 +3456,13 @@
       <c r="M21" s="22"/>
       <c r="N21" s="22"/>
       <c r="O21" s="22"/>
-      <c r="P21" s="61"/>
-      <c r="Q21" s="44"/>
-    </row>
-    <row r="22" spans="2:18" ht="14.25" customHeight="1">
-      <c r="B22" s="62"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="93" t="s">
+      <c r="P21" s="93"/>
+      <c r="Q21" s="54"/>
+    </row>
+    <row r="22" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="82"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="40" t="s">
         <v>25</v>
       </c>
       <c r="E22" s="9"/>
@@ -3482,13 +3477,13 @@
       <c r="M22" s="22"/>
       <c r="N22" s="22"/>
       <c r="O22" s="22"/>
-      <c r="P22" s="61"/>
-      <c r="Q22" s="44"/>
-    </row>
-    <row r="23" spans="2:18" ht="14.25" customHeight="1">
-      <c r="B23" s="62"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="93" t="s">
+      <c r="P22" s="93"/>
+      <c r="Q22" s="54"/>
+    </row>
+    <row r="23" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="82"/>
+      <c r="C23" s="82"/>
+      <c r="D23" s="40" t="s">
         <v>25</v>
       </c>
       <c r="E23" s="9"/>
@@ -3503,13 +3498,13 @@
       <c r="M23" s="22"/>
       <c r="N23" s="22"/>
       <c r="O23" s="22"/>
-      <c r="P23" s="61"/>
-      <c r="Q23" s="44"/>
-    </row>
-    <row r="24" spans="2:18" ht="14.25" customHeight="1">
-      <c r="B24" s="55"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="93" t="s">
+      <c r="P23" s="93"/>
+      <c r="Q23" s="54"/>
+    </row>
+    <row r="24" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="76"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="40" t="s">
         <v>25</v>
       </c>
       <c r="E24" s="9"/>
@@ -3524,14 +3519,14 @@
       <c r="M24" s="22"/>
       <c r="N24" s="22"/>
       <c r="O24" s="22"/>
-      <c r="P24" s="61"/>
-      <c r="Q24" s="44"/>
-    </row>
-    <row r="25" spans="2:18" ht="14.25" customHeight="1">
-      <c r="B25" s="54">
+      <c r="P24" s="93"/>
+      <c r="Q24" s="54"/>
+    </row>
+    <row r="25" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="75">
         <v>4</v>
       </c>
-      <c r="C25" s="63" t="s">
+      <c r="C25" s="83" t="s">
         <v>25</v>
       </c>
       <c r="D25" s="12" t="s">
@@ -3549,12 +3544,12 @@
       <c r="M25" s="22"/>
       <c r="N25" s="22"/>
       <c r="O25" s="22"/>
-      <c r="P25" s="61"/>
-      <c r="Q25" s="44"/>
-    </row>
-    <row r="26" spans="2:18" ht="14.25" customHeight="1">
-      <c r="B26" s="62"/>
-      <c r="C26" s="62"/>
+      <c r="P25" s="93"/>
+      <c r="Q25" s="54"/>
+    </row>
+    <row r="26" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="82"/>
+      <c r="C26" s="82"/>
       <c r="D26" s="12" t="s">
         <v>25</v>
       </c>
@@ -3572,9 +3567,9 @@
       <c r="Q26" s="9"/>
       <c r="R26" s="9"/>
     </row>
-    <row r="27" spans="2:18" ht="14.25" customHeight="1">
-      <c r="B27" s="62"/>
-      <c r="C27" s="62"/>
+    <row r="27" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="82"/>
+      <c r="C27" s="82"/>
       <c r="D27" s="12" t="s">
         <v>25</v>
       </c>
@@ -3592,49 +3587,49 @@
       <c r="Q27" s="9"/>
       <c r="R27" s="9"/>
     </row>
-    <row r="28" spans="2:18" ht="14.25" customHeight="1">
-      <c r="B28" s="62"/>
-      <c r="C28" s="62"/>
+    <row r="28" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="82"/>
+      <c r="C28" s="82"/>
       <c r="D28" s="12" t="s">
         <v>25</v>
       </c>
       <c r="E28" s="9"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="41"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="41"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="92"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="51"/>
+      <c r="L28" s="51"/>
+      <c r="M28" s="51"/>
       <c r="N28" s="27"/>
       <c r="O28" s="9"/>
       <c r="P28" s="9"/>
       <c r="Q28" s="9"/>
       <c r="R28" s="9"/>
     </row>
-    <row r="29" spans="2:18" ht="14.25" customHeight="1">
-      <c r="B29" s="62"/>
-      <c r="C29" s="62"/>
+    <row r="29" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="82"/>
+      <c r="C29" s="82"/>
       <c r="D29" s="12" t="s">
         <v>25</v>
       </c>
       <c r="E29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
-      <c r="I29" s="64"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="41"/>
-      <c r="M29" s="41"/>
+      <c r="I29" s="91"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="51"/>
+      <c r="L29" s="51"/>
+      <c r="M29" s="51"/>
       <c r="N29" s="28"/>
       <c r="O29" s="9"/>
       <c r="P29" s="9"/>
       <c r="Q29" s="9"/>
       <c r="R29" s="9"/>
     </row>
-    <row r="30" spans="2:18" ht="14.25" customHeight="1">
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
+    <row r="30" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="76"/>
+      <c r="C30" s="76"/>
       <c r="D30" s="12" t="s">
         <v>25</v>
       </c>
@@ -3647,7 +3642,7 @@
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
     </row>
-    <row r="31" spans="2:18" ht="14.25" customHeight="1">
+    <row r="31" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
@@ -3656,103 +3651,77 @@
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
     </row>
-    <row r="32" spans="2:18" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
+    <row r="32" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B7:B12"/>
-    <mergeCell ref="C7:C12"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="G5:Q5"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="B13:B18"/>
-    <mergeCell ref="C13:C18"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="I29:M29"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:M28"/>
-    <mergeCell ref="B25:B30"/>
-    <mergeCell ref="C25:C30"/>
     <mergeCell ref="P20:Q20"/>
     <mergeCell ref="P12:Q12"/>
     <mergeCell ref="P13:Q13"/>
@@ -3767,6 +3736,32 @@
     <mergeCell ref="P17:Q17"/>
     <mergeCell ref="P18:Q18"/>
     <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="B13:B18"/>
+    <mergeCell ref="C13:C18"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="B19:B24"/>
+    <mergeCell ref="I29:M29"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:M28"/>
+    <mergeCell ref="B25:B30"/>
+    <mergeCell ref="C25:C30"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="C7:C12"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="G5:Q5"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="G6:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -3775,17 +3770,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF666699"/>
   </sheetPr>
   <dimension ref="B1:O100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
@@ -3798,405 +3793,405 @@
     <col min="13" max="14" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="14.25" customHeight="1">
+    <row r="1" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="9"/>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="2" spans="2:15" ht="14.25" customHeight="1"/>
-    <row r="3" spans="2:15" ht="14.25" customHeight="1">
-      <c r="B3" s="129" t="s">
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="54"/>
+    </row>
+    <row r="2" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="130"/>
-      <c r="D3" s="130"/>
-      <c r="E3" s="130"/>
-      <c r="F3" s="130"/>
-      <c r="G3" s="130"/>
-      <c r="H3" s="130"/>
-      <c r="I3" s="130"/>
-      <c r="J3" s="130"/>
-      <c r="K3" s="130"/>
-      <c r="L3" s="130"/>
-      <c r="M3" s="130"/>
-      <c r="N3" s="130"/>
-    </row>
-    <row r="4" spans="2:15" ht="14.25" customHeight="1">
-      <c r="B4" s="57" t="s">
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+    </row>
+    <row r="4" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="68" t="s">
+      <c r="C4" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="128" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="127" t="s">
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="128"/>
-      <c r="M4" s="128"/>
-      <c r="N4" s="128"/>
-      <c r="O4" s="128"/>
-    </row>
-    <row r="5" spans="2:15" ht="14.25" customHeight="1" thickBot="1">
-      <c r="B5" s="86"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="86"/>
+      <c r="L4" s="98"/>
+      <c r="M4" s="98"/>
+      <c r="N4" s="98"/>
+      <c r="O4" s="98"/>
+    </row>
+    <row r="5" spans="2:15" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="127"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="127"/>
       <c r="F5" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="I5" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="J5" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="J5" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="K5" s="91" t="s">
+      <c r="K5" s="125" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="124"/>
-      <c r="M5" s="127" t="s">
-        <v>116</v>
-      </c>
-      <c r="N5" s="128"/>
-    </row>
-    <row r="6" spans="2:15" ht="14.25" customHeight="1" thickTop="1">
+      <c r="L5" s="126"/>
+      <c r="M5" s="97" t="s">
+        <v>114</v>
+      </c>
+      <c r="N5" s="98"/>
+    </row>
+    <row r="6" spans="2:15" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B6" s="30">
         <v>1</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="122" t="s">
         <v>47</v>
       </c>
       <c r="D6" s="10">
         <v>1</v>
       </c>
-      <c r="E6" s="99"/>
-      <c r="F6" s="99" t="s">
+      <c r="E6" s="43"/>
+      <c r="F6" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98">
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42">
         <v>3301</v>
       </c>
-      <c r="K6" s="52" t="b">
+      <c r="K6" s="67" t="b">
         <v>1</v>
       </c>
-      <c r="L6" s="96"/>
-      <c r="M6" s="112" t="b">
+      <c r="L6" s="66"/>
+      <c r="M6" s="61" t="b">
         <v>1</v>
       </c>
-      <c r="N6" s="113"/>
+      <c r="N6" s="62"/>
       <c r="O6" s="9"/>
     </row>
-    <row r="7" spans="2:15" ht="14.25" customHeight="1">
+    <row r="7" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
         <f t="shared" ref="B7:B13" si="0">B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="84"/>
+      <c r="C7" s="123"/>
       <c r="D7" s="10">
         <v>2</v>
       </c>
-      <c r="E7" s="99"/>
-      <c r="F7" s="99" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" s="98"/>
-      <c r="H7" s="98"/>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98">
+      <c r="E7" s="43"/>
+      <c r="F7" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42">
         <v>3301</v>
       </c>
-      <c r="K7" s="112" t="b">
+      <c r="K7" s="61" t="b">
         <v>1</v>
       </c>
-      <c r="L7" s="113"/>
-      <c r="M7" s="112" t="b">
+      <c r="L7" s="62"/>
+      <c r="M7" s="61" t="b">
         <v>1</v>
       </c>
-      <c r="N7" s="113"/>
+      <c r="N7" s="62"/>
       <c r="O7" s="9"/>
     </row>
-    <row r="8" spans="2:15" ht="14.25" customHeight="1">
+    <row r="8" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C8" s="84"/>
+      <c r="C8" s="123"/>
       <c r="D8" s="13">
         <v>3</v>
       </c>
-      <c r="E8" s="99"/>
-      <c r="F8" s="98" t="s">
-        <v>60</v>
+      <c r="E8" s="43"/>
+      <c r="F8" s="42" t="s">
+        <v>59</v>
       </c>
       <c r="G8" s="17"/>
-      <c r="H8" s="98"/>
-      <c r="I8" s="98"/>
-      <c r="J8" s="98">
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42">
         <v>3301</v>
       </c>
-      <c r="K8" s="112" t="b">
+      <c r="K8" s="61" t="b">
         <v>0</v>
       </c>
-      <c r="L8" s="113"/>
-      <c r="M8" s="112" t="b">
+      <c r="L8" s="62"/>
+      <c r="M8" s="61" t="b">
         <v>0</v>
       </c>
-      <c r="N8" s="113"/>
+      <c r="N8" s="62"/>
       <c r="O8" s="9"/>
     </row>
-    <row r="9" spans="2:15" ht="14.25" customHeight="1">
+    <row r="9" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C9" s="84"/>
+      <c r="C9" s="123"/>
       <c r="D9" s="13">
         <v>4</v>
       </c>
-      <c r="E9" s="99"/>
-      <c r="F9" s="98" t="s">
-        <v>80</v>
-      </c>
-      <c r="G9" s="98"/>
-      <c r="H9" s="98"/>
-      <c r="I9" s="98"/>
-      <c r="J9" s="98">
+      <c r="E9" s="43"/>
+      <c r="F9" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42">
         <v>3300</v>
       </c>
-      <c r="K9" s="112" t="b">
+      <c r="K9" s="61" t="b">
         <v>0</v>
       </c>
-      <c r="L9" s="113"/>
-      <c r="M9" s="112" t="b">
+      <c r="L9" s="62"/>
+      <c r="M9" s="61" t="b">
         <v>0</v>
       </c>
-      <c r="N9" s="113"/>
+      <c r="N9" s="62"/>
       <c r="O9" s="9"/>
     </row>
-    <row r="10" spans="2:15" ht="14.25" customHeight="1">
+    <row r="10" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C10" s="84"/>
+      <c r="C10" s="123"/>
       <c r="D10" s="14">
         <v>5</v>
       </c>
-      <c r="E10" s="99"/>
-      <c r="F10" s="98" t="s">
+      <c r="E10" s="43"/>
+      <c r="F10" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="98"/>
-      <c r="H10" s="98"/>
-      <c r="I10" s="98"/>
-      <c r="J10" s="98">
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42">
         <v>3300</v>
       </c>
-      <c r="K10" s="112" t="b">
+      <c r="K10" s="61" t="b">
         <v>0</v>
       </c>
-      <c r="L10" s="113"/>
-      <c r="M10" s="112" t="b">
+      <c r="L10" s="62"/>
+      <c r="M10" s="61" t="b">
         <v>0</v>
       </c>
-      <c r="N10" s="113"/>
+      <c r="N10" s="62"/>
       <c r="O10" s="9"/>
     </row>
-    <row r="11" spans="2:15" ht="14.25" customHeight="1">
+    <row r="11" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C11" s="84"/>
+      <c r="C11" s="123"/>
       <c r="D11" s="14">
         <v>6</v>
       </c>
-      <c r="E11" s="99"/>
-      <c r="F11" s="99" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="98"/>
-      <c r="H11" s="99"/>
-      <c r="I11" s="98"/>
-      <c r="J11" s="98" t="s">
-        <v>114</v>
-      </c>
-      <c r="K11" s="112" t="b">
+      <c r="E11" s="43"/>
+      <c r="F11" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="42"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="K11" s="61" t="b">
         <v>0</v>
       </c>
-      <c r="L11" s="113"/>
-      <c r="M11" s="112" t="b">
+      <c r="L11" s="62"/>
+      <c r="M11" s="61" t="b">
         <v>0</v>
       </c>
-      <c r="N11" s="113"/>
+      <c r="N11" s="62"/>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="2:15" ht="14.25" customHeight="1">
+    <row r="12" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C12" s="84"/>
+      <c r="C12" s="123"/>
       <c r="D12" s="15">
         <v>7</v>
       </c>
-      <c r="E12" s="99"/>
-      <c r="F12" s="99" t="s">
-        <v>80</v>
-      </c>
-      <c r="G12" s="98"/>
-      <c r="H12" s="98"/>
-      <c r="I12" s="98"/>
-      <c r="J12" s="98">
+      <c r="E12" s="43"/>
+      <c r="F12" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42">
         <v>12000</v>
       </c>
-      <c r="K12" s="112" t="b">
+      <c r="K12" s="61" t="b">
         <v>0</v>
       </c>
-      <c r="L12" s="113"/>
-      <c r="M12" s="112" t="b">
+      <c r="L12" s="62"/>
+      <c r="M12" s="61" t="b">
         <v>0</v>
       </c>
-      <c r="N12" s="113"/>
+      <c r="N12" s="62"/>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="2:15" ht="14.25" customHeight="1" thickBot="1">
+    <row r="13" spans="2:15" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="29">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C13" s="85"/>
+      <c r="C13" s="124"/>
       <c r="D13" s="15">
         <v>8</v>
       </c>
-      <c r="E13" s="99"/>
-      <c r="F13" s="99" t="s">
-        <v>81</v>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43" t="s">
+        <v>80</v>
       </c>
       <c r="G13" s="24"/>
-      <c r="H13" s="100"/>
+      <c r="H13" s="44"/>
       <c r="I13" s="24"/>
-      <c r="J13" s="100">
+      <c r="J13" s="44">
         <v>8000</v>
       </c>
-      <c r="K13" s="112" t="b">
+      <c r="K13" s="61" t="b">
         <v>0</v>
       </c>
-      <c r="L13" s="113"/>
-      <c r="M13" s="112" t="b">
+      <c r="L13" s="62"/>
+      <c r="M13" s="61" t="b">
         <v>0</v>
       </c>
-      <c r="N13" s="113"/>
+      <c r="N13" s="62"/>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="2:15" ht="14.25" customHeight="1" thickTop="1" thickBot="1">
+    <row r="14" spans="2:15" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="29"/>
-      <c r="C14" s="83" t="s">
+      <c r="C14" s="122" t="s">
         <v>47</v>
       </c>
       <c r="D14" s="10"/>
-      <c r="E14" s="99"/>
-      <c r="F14" s="99"/>
-      <c r="G14" s="98"/>
-      <c r="H14" s="98"/>
-      <c r="I14" s="98"/>
-      <c r="J14" s="98"/>
-      <c r="K14" s="112"/>
-      <c r="L14" s="113"/>
-      <c r="M14" s="112"/>
-      <c r="N14" s="113"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="61"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="61"/>
+      <c r="N14" s="62"/>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="2:15" ht="14.25" customHeight="1" thickTop="1">
+    <row r="15" spans="2:15" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>10</v>
       </c>
-      <c r="C15" s="119"/>
+      <c r="C15" s="130"/>
       <c r="D15" s="20"/>
       <c r="E15" s="20">
         <v>1</v>
       </c>
-      <c r="F15" s="122" t="s">
+      <c r="F15" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="94"/>
+      <c r="G15" s="41"/>
       <c r="H15" s="22"/>
       <c r="I15" s="22"/>
       <c r="J15" s="22">
         <v>3302</v>
       </c>
-      <c r="K15" s="125" t="b">
+      <c r="K15" s="95" t="b">
         <v>0</v>
       </c>
-      <c r="L15" s="126"/>
-      <c r="M15" s="125" t="b">
+      <c r="L15" s="96"/>
+      <c r="M15" s="95" t="b">
         <v>0</v>
       </c>
-      <c r="N15" s="126"/>
+      <c r="N15" s="96"/>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="2:15" ht="14.25" customHeight="1">
+    <row r="16" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="15">
         <v>11</v>
       </c>
-      <c r="C16" s="84"/>
+      <c r="C16" s="123"/>
       <c r="D16" s="23"/>
       <c r="E16" s="23">
         <v>2</v>
       </c>
-      <c r="F16" s="107" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="107"/>
+      <c r="F16" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="47"/>
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
       <c r="J16" s="22">
         <v>3302</v>
       </c>
-      <c r="K16" s="125" t="s">
-        <v>115</v>
-      </c>
-      <c r="L16" s="126"/>
-      <c r="M16" s="125" t="s">
-        <v>115</v>
-      </c>
-      <c r="N16" s="126"/>
+      <c r="K16" s="95" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" s="96"/>
+      <c r="M16" s="95" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16" s="96"/>
       <c r="O16" s="9"/>
     </row>
-    <row r="17" spans="2:14" ht="14.25" customHeight="1">
+    <row r="17" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>12</v>
       </c>
-      <c r="C17" s="84"/>
+      <c r="C17" s="123"/>
       <c r="D17" s="20"/>
       <c r="E17" s="20">
         <v>3</v>
@@ -4210,20 +4205,20 @@
       <c r="J17" s="22">
         <v>3302</v>
       </c>
-      <c r="K17" s="118" t="b">
+      <c r="K17" s="63" t="b">
         <v>1</v>
       </c>
-      <c r="L17" s="101"/>
-      <c r="M17" s="118" t="b">
+      <c r="L17" s="64"/>
+      <c r="M17" s="63" t="b">
         <v>1</v>
       </c>
-      <c r="N17" s="101"/>
-    </row>
-    <row r="18" spans="2:14" ht="14.25" customHeight="1">
+      <c r="N17" s="64"/>
+    </row>
+    <row r="18" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>13</v>
       </c>
-      <c r="C18" s="84"/>
+      <c r="C18" s="123"/>
       <c r="D18" s="20"/>
       <c r="E18" s="20">
         <v>4</v>
@@ -4237,20 +4232,20 @@
       <c r="J18" s="22">
         <v>3302</v>
       </c>
-      <c r="K18" s="118" t="b">
+      <c r="K18" s="63" t="b">
         <v>1</v>
       </c>
-      <c r="L18" s="101"/>
-      <c r="M18" s="118" t="b">
+      <c r="L18" s="64"/>
+      <c r="M18" s="63" t="b">
         <v>1</v>
       </c>
-      <c r="N18" s="101"/>
-    </row>
-    <row r="19" spans="2:14" ht="14.25" customHeight="1">
+      <c r="N18" s="64"/>
+    </row>
+    <row r="19" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>14</v>
       </c>
-      <c r="C19" s="84"/>
+      <c r="C19" s="123"/>
       <c r="D19" s="20"/>
       <c r="E19" s="20">
         <v>5</v>
@@ -4264,20 +4259,20 @@
       <c r="J19" s="22">
         <v>3302</v>
       </c>
-      <c r="K19" s="118" t="b">
+      <c r="K19" s="63" t="b">
         <v>1</v>
       </c>
-      <c r="L19" s="101"/>
-      <c r="M19" s="118" t="b">
+      <c r="L19" s="64"/>
+      <c r="M19" s="63" t="b">
         <v>1</v>
       </c>
-      <c r="N19" s="101"/>
-    </row>
-    <row r="20" spans="2:14" ht="14.25" customHeight="1">
+      <c r="N19" s="64"/>
+    </row>
+    <row r="20" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="15">
         <v>15</v>
       </c>
-      <c r="C20" s="84"/>
+      <c r="C20" s="123"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23">
         <v>6</v>
@@ -4291,196 +4286,196 @@
       <c r="J20" s="22">
         <v>3302</v>
       </c>
-      <c r="K20" s="114" t="b">
+      <c r="K20" s="101" t="b">
         <v>0</v>
       </c>
-      <c r="L20" s="115"/>
-      <c r="M20" s="114" t="b">
+      <c r="L20" s="102"/>
+      <c r="M20" s="101" t="b">
         <v>0</v>
       </c>
-      <c r="N20" s="115"/>
-    </row>
-    <row r="21" spans="2:14" ht="14.25" customHeight="1" thickBot="1">
+      <c r="N20" s="102"/>
+    </row>
+    <row r="21" spans="2:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="10">
         <v>16</v>
       </c>
-      <c r="C21" s="85"/>
+      <c r="C21" s="124"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20">
         <v>7</v>
       </c>
-      <c r="F21" s="94" t="s">
-        <v>80</v>
-      </c>
-      <c r="G21" s="94"/>
+      <c r="F21" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="41"/>
       <c r="H21" s="22"/>
       <c r="I21" s="22"/>
-      <c r="J21" s="122">
+      <c r="J21" s="48">
         <v>3300</v>
       </c>
-      <c r="K21" s="114" t="b">
+      <c r="K21" s="101" t="b">
         <v>0</v>
       </c>
-      <c r="L21" s="115"/>
-      <c r="M21" s="114" t="b">
+      <c r="L21" s="102"/>
+      <c r="M21" s="101" t="b">
         <v>0</v>
       </c>
-      <c r="N21" s="115"/>
-    </row>
-    <row r="22" spans="2:14" ht="14.25" customHeight="1" thickTop="1">
+      <c r="N21" s="102"/>
+    </row>
+    <row r="22" spans="2:14" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>17</v>
       </c>
-      <c r="C22" s="83" t="s">
+      <c r="C22" s="122" t="s">
         <v>47</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="20">
         <v>8</v>
       </c>
-      <c r="F22" s="94" t="s">
-        <v>80</v>
-      </c>
-      <c r="G22" s="94"/>
+      <c r="F22" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="41"/>
       <c r="H22" s="22"/>
       <c r="I22" s="22"/>
       <c r="J22" s="22">
         <v>3301</v>
       </c>
-      <c r="K22" s="118" t="b">
+      <c r="K22" s="63" t="b">
         <v>1</v>
       </c>
-      <c r="L22" s="101"/>
-      <c r="M22" s="118" t="b">
+      <c r="L22" s="64"/>
+      <c r="M22" s="63" t="b">
         <v>1</v>
       </c>
-      <c r="N22" s="101"/>
-    </row>
-    <row r="23" spans="2:14" ht="14.25" customHeight="1">
+      <c r="N22" s="64"/>
+    </row>
+    <row r="23" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10">
         <v>18</v>
       </c>
-      <c r="C23" s="84"/>
+      <c r="C23" s="123"/>
       <c r="D23" s="20"/>
       <c r="E23" s="20">
         <v>9</v>
       </c>
-      <c r="F23" s="94" t="s">
-        <v>80</v>
-      </c>
-      <c r="G23" s="94"/>
+      <c r="F23" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="41"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="22">
         <v>3302</v>
       </c>
-      <c r="K23" s="118" t="b">
+      <c r="K23" s="63" t="b">
         <v>1</v>
       </c>
-      <c r="L23" s="101"/>
-      <c r="M23" s="118" t="b">
+      <c r="L23" s="64"/>
+      <c r="M23" s="63" t="b">
         <v>1</v>
       </c>
-      <c r="N23" s="101"/>
-    </row>
-    <row r="24" spans="2:14" ht="14.25" customHeight="1">
+      <c r="N23" s="64"/>
+    </row>
+    <row r="24" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10">
         <v>19</v>
       </c>
-      <c r="C24" s="84"/>
+      <c r="C24" s="123"/>
       <c r="D24" s="20"/>
       <c r="E24" s="20">
         <v>10</v>
       </c>
-      <c r="F24" s="94" t="s">
-        <v>80</v>
-      </c>
-      <c r="G24" s="94"/>
+      <c r="F24" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="41"/>
       <c r="H24" s="22"/>
       <c r="I24" s="22"/>
       <c r="J24" s="22">
         <v>11998</v>
       </c>
-      <c r="K24" s="118" t="b">
+      <c r="K24" s="63" t="b">
         <v>1</v>
       </c>
-      <c r="L24" s="101"/>
-      <c r="M24" s="118" t="b">
+      <c r="L24" s="64"/>
+      <c r="M24" s="63" t="b">
         <v>1</v>
       </c>
-      <c r="N24" s="101"/>
-    </row>
-    <row r="25" spans="2:14" ht="14.25" customHeight="1">
+      <c r="N24" s="64"/>
+    </row>
+    <row r="25" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10">
         <v>20</v>
       </c>
-      <c r="C25" s="84"/>
+      <c r="C25" s="123"/>
       <c r="D25" s="20"/>
       <c r="E25" s="20">
         <v>11</v>
       </c>
-      <c r="F25" s="94" t="s">
-        <v>80</v>
-      </c>
-      <c r="G25" s="94"/>
+      <c r="F25" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="41"/>
       <c r="H25" s="22"/>
       <c r="I25" s="22"/>
       <c r="J25" s="22">
         <v>11999</v>
       </c>
-      <c r="K25" s="118" t="b">
+      <c r="K25" s="63" t="b">
         <v>1</v>
       </c>
-      <c r="L25" s="101"/>
-      <c r="M25" s="118" t="b">
+      <c r="L25" s="64"/>
+      <c r="M25" s="63" t="b">
         <v>1</v>
       </c>
-      <c r="N25" s="101"/>
-    </row>
-    <row r="26" spans="2:14" ht="14.25" customHeight="1">
+      <c r="N25" s="64"/>
+    </row>
+    <row r="26" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10">
         <v>21</v>
       </c>
-      <c r="C26" s="84"/>
+      <c r="C26" s="123"/>
       <c r="D26" s="20"/>
       <c r="E26" s="20">
         <v>12</v>
       </c>
-      <c r="F26" s="94" t="s">
-        <v>80</v>
-      </c>
-      <c r="G26" s="94"/>
+      <c r="F26" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="41"/>
       <c r="H26" s="22"/>
       <c r="I26" s="22"/>
-      <c r="J26" s="122">
+      <c r="J26" s="48">
         <v>12000</v>
       </c>
-      <c r="K26" s="125" t="b">
+      <c r="K26" s="95" t="b">
         <v>0</v>
       </c>
-      <c r="L26" s="126"/>
-      <c r="M26" s="125" t="b">
+      <c r="L26" s="96"/>
+      <c r="M26" s="95" t="b">
         <v>0</v>
       </c>
-      <c r="N26" s="126"/>
-    </row>
-    <row r="27" spans="2:14" ht="14.25" customHeight="1">
-      <c r="C27" s="84"/>
-    </row>
-    <row r="28" spans="2:14" ht="14.25" customHeight="1">
-      <c r="C28" s="84"/>
-    </row>
-    <row r="29" spans="2:14" ht="14.25" customHeight="1" thickBot="1">
-      <c r="C29" s="85"/>
-    </row>
-    <row r="30" spans="2:14" ht="14.25" customHeight="1" thickTop="1"/>
-    <row r="31" spans="2:14" ht="14.25" customHeight="1"/>
-    <row r="32" spans="2:14" ht="14.25" customHeight="1">
+      <c r="N26" s="96"/>
+    </row>
+    <row r="27" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="123"/>
+    </row>
+    <row r="28" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="123"/>
+    </row>
+    <row r="29" spans="2:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="124"/>
+    </row>
+    <row r="30" spans="2:14" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="31" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="2:14" ht="14.25" customHeight="1">
+    <row r="33" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="9"/>
       <c r="C33" s="31"/>
       <c r="D33" s="31"/>
@@ -4495,7 +4490,7 @@
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
     </row>
-    <row r="34" spans="2:14" ht="14.25" customHeight="1" thickBot="1">
+    <row r="34" spans="2:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -4510,176 +4505,243 @@
       <c r="M34" s="9"/>
       <c r="N34" s="9"/>
     </row>
-    <row r="35" spans="2:14" ht="14.25" customHeight="1" thickTop="1">
-      <c r="B35" s="89" t="s">
+    <row r="35" spans="2:14" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="70" t="s">
+      <c r="C35" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="120"/>
-      <c r="E35" s="120"/>
-      <c r="F35" s="121"/>
+      <c r="D35" s="118"/>
+      <c r="E35" s="118"/>
+      <c r="F35" s="119"/>
       <c r="G35" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="H35" s="70" t="s">
+      <c r="H35" s="117" t="s">
         <v>51</v>
       </c>
-      <c r="I35" s="71"/>
-      <c r="J35" s="71"/>
-      <c r="K35" s="70" t="s">
+      <c r="I35" s="120"/>
+      <c r="J35" s="120"/>
+      <c r="K35" s="117" t="s">
         <v>52</v>
       </c>
-      <c r="L35" s="71"/>
-      <c r="M35" s="71"/>
-      <c r="N35" s="72"/>
-    </row>
-    <row r="36" spans="2:14" ht="14.25" customHeight="1">
-      <c r="B36" s="90"/>
-      <c r="C36" s="80" t="s">
+      <c r="L35" s="120"/>
+      <c r="M35" s="120"/>
+      <c r="N35" s="121"/>
+    </row>
+    <row r="36" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="115"/>
+      <c r="C36" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="D36" s="57" t="s">
+      <c r="D36" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="57" t="s">
+      <c r="E36" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="F36" s="68" t="s">
+      <c r="F36" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="G36" s="81" t="s">
+      <c r="G36" s="108" t="s">
         <v>57</v>
       </c>
-      <c r="H36" s="73" t="s">
+      <c r="H36" s="110" t="s">
         <v>58</v>
       </c>
-      <c r="I36" s="74"/>
-      <c r="J36" s="57" t="s">
+      <c r="I36" s="111"/>
+      <c r="J36" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="K36" s="78" t="s">
+      <c r="K36" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="L36" s="57" t="s">
+      <c r="L36" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="M36" s="57" t="s">
+      <c r="M36" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="N36" s="68" t="s">
+      <c r="N36" s="105" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="2:14" ht="14.25" customHeight="1">
+    <row r="37" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="79"/>
-      <c r="D37" s="55"/>
-      <c r="E37" s="55"/>
-      <c r="F37" s="69"/>
-      <c r="G37" s="82"/>
-      <c r="H37" s="75"/>
-      <c r="I37" s="76"/>
-      <c r="J37" s="55"/>
-      <c r="K37" s="79"/>
-      <c r="L37" s="55"/>
-      <c r="M37" s="55"/>
-      <c r="N37" s="69"/>
-    </row>
-    <row r="38" spans="2:14" ht="14.25" customHeight="1">
+      <c r="C37" s="104"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="76"/>
+      <c r="F37" s="106"/>
+      <c r="G37" s="109"/>
+      <c r="H37" s="112"/>
+      <c r="I37" s="113"/>
+      <c r="J37" s="76"/>
+      <c r="K37" s="104"/>
+      <c r="L37" s="76"/>
+      <c r="M37" s="76"/>
+      <c r="N37" s="106"/>
+    </row>
+    <row r="38" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="35">
         <f>SUM(D38:E38)</f>
+        <v>12</v>
+      </c>
+      <c r="D38" s="36">
+        <v>12</v>
+      </c>
+      <c r="E38" s="36">
         <v>0</v>
       </c>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="77" t="s">
-        <v>59</v>
-      </c>
-      <c r="I38" s="44"/>
+      <c r="F38" s="37">
+        <v>0</v>
+      </c>
+      <c r="G38" s="38">
+        <v>0</v>
+      </c>
+      <c r="H38" s="107">
+        <v>12</v>
+      </c>
+      <c r="I38" s="54"/>
       <c r="J38" s="12" t="e">
         <f>SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="K38" s="39" t="s">
-        <v>59</v>
+      <c r="K38" s="39">
+        <v>12</v>
       </c>
       <c r="L38" s="12">
         <f>SUM(M38:N38)</f>
+        <v>12</v>
+      </c>
+      <c r="M38" s="36">
+        <v>12</v>
+      </c>
+      <c r="N38" s="37">
         <v>0</v>
       </c>
-      <c r="M38" s="36"/>
-      <c r="N38" s="37"/>
-    </row>
-    <row r="39" spans="2:14" ht="14.25" customHeight="1"/>
-    <row r="40" spans="2:14" ht="14.25" customHeight="1"/>
-    <row r="41" spans="2:14" ht="14.25" customHeight="1"/>
-    <row r="42" spans="2:14" ht="14.25" customHeight="1"/>
-    <row r="43" spans="2:14" ht="14.25" customHeight="1"/>
-    <row r="44" spans="2:14" ht="14.25" customHeight="1"/>
-    <row r="45" spans="2:14" ht="14.25" customHeight="1"/>
-    <row r="46" spans="2:14" ht="14.25" customHeight="1"/>
-    <row r="47" spans="2:14" ht="14.25" customHeight="1"/>
-    <row r="48" spans="2:14" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
+    </row>
+    <row r="39" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="71">
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K35:N35"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="C22:C29"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="C14:C21"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="H36:I37"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
     <mergeCell ref="M26:N26"/>
     <mergeCell ref="K4:O4"/>
     <mergeCell ref="B3:N3"/>
@@ -4696,61 +4758,6 @@
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="M7:N7"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K36:K37"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="H36:I37"/>
-    <mergeCell ref="J36:J37"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="K35:N35"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="C22:C29"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C14:C21"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M13:N13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>